<commit_message>
Added SPIN Count to Jackpot log
Added total reel stops to spreadsheet
</commit_message>
<xml_diff>
--- a/Odds Calculator.xlsx
+++ b/Odds Calculator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicholas.wautier\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas.Wautier\Documents\GitHub\ASCII-Slot\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Reel 1</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>:Multiplyer for 3</t>
+  </si>
+  <si>
+    <t>:Total Spin Possibilities</t>
   </si>
 </sst>
 </file>
@@ -127,9 +130,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -138,6 +138,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,6 +447,7 @@
     <col min="23" max="23" width="5" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="6" hidden="1" customWidth="1"/>
     <col min="25" max="26" width="0" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -459,11 +463,11 @@
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
       <c r="N2" t="s">
         <v>3</v>
       </c>
@@ -493,57 +497,57 @@
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3">
-        <f>COUNTIF(A:A,E3)</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
-        <f>COUNTIF(B:B,E3)</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="3">
-        <f>COUNTIF(C:C,E3)</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4">
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F13" si="0">COUNTIF(A:A,E3)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G13" si="1">COUNTIF(B:B,E3)</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <f t="shared" ref="H3:H13" si="2">COUNTIF(C:C,E3)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3">
         <f>F3/SUM($F$3:$F$13)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="3">
         <f>G3/SUM($G$3:$G$13)</f>
         <v>0</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="3">
         <f>H3/SUM($H$3:$H$13)</f>
         <v>0</v>
       </c>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4">
+      <c r="M3" s="3"/>
+      <c r="N3" s="3">
         <f>J3</f>
         <v>0</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O3" s="3">
         <f>J3*K3</f>
         <v>0</v>
       </c>
-      <c r="P3" s="4">
+      <c r="P3" s="3">
         <f>J3*K3*L3</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4">
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3">
         <f>E3*$R$14</f>
         <v>0</v>
       </c>
-      <c r="S3" s="4">
+      <c r="S3" s="3">
         <f>E3*$S$14</f>
         <v>0</v>
       </c>
-      <c r="T3" s="4">
+      <c r="T3" s="3">
         <f>E3*$T$14</f>
         <v>0</v>
       </c>
@@ -570,62 +574,62 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="5">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5">
-        <f>COUNTIF(A:A,E4)</f>
-        <v>1</v>
-      </c>
-      <c r="G4" s="5">
-        <f>COUNTIF(B:B,E4)</f>
-        <v>1</v>
-      </c>
-      <c r="H4" s="5">
-        <f>COUNTIF(C:C,E4)</f>
-        <v>1</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6">
-        <f t="shared" ref="J4:J13" si="0">F4/SUM($F$3:$F$13)</f>
-        <v>0.1</v>
-      </c>
-      <c r="K4" s="6">
-        <f t="shared" ref="K4:K13" si="1">G4/SUM($G$3:$G$13)</f>
-        <v>0.1</v>
-      </c>
-      <c r="L4" s="6">
-        <f t="shared" ref="L4:L13" si="2">H4/SUM($H$3:$H$13)</f>
-        <v>0.1</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6">
-        <f t="shared" ref="N4:N12" si="3">J4</f>
-        <v>0.1</v>
-      </c>
-      <c r="O4" s="6">
-        <f t="shared" ref="O4:O12" si="4">J4*K4</f>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H4" s="4">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5">
+        <f t="shared" ref="J4:J13" si="3">F4/SUM($F$3:$F$13)</f>
+        <v>0.1</v>
+      </c>
+      <c r="K4" s="5">
+        <f t="shared" ref="K4:K13" si="4">G4/SUM($G$3:$G$13)</f>
+        <v>0.1</v>
+      </c>
+      <c r="L4" s="5">
+        <f t="shared" ref="L4:L13" si="5">H4/SUM($H$3:$H$13)</f>
+        <v>0.1</v>
+      </c>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5">
+        <f t="shared" ref="N4:N12" si="6">J4</f>
+        <v>0.1</v>
+      </c>
+      <c r="O4" s="5">
+        <f t="shared" ref="O4:O12" si="7">J4*K4</f>
         <v>1.0000000000000002E-2</v>
       </c>
-      <c r="P4" s="6">
-        <f t="shared" ref="P4:P12" si="5">J4*K4*L4</f>
+      <c r="P4" s="5">
+        <f t="shared" ref="P4:P12" si="8">J4*K4*L4</f>
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6">
-        <f t="shared" ref="R4:R12" si="6">E4*$R$14</f>
-        <v>0</v>
-      </c>
-      <c r="S4" s="6">
-        <f t="shared" ref="S4:S12" si="7">E4*$S$14</f>
-        <v>1</v>
-      </c>
-      <c r="T4" s="6">
-        <f t="shared" ref="T4:T12" si="8">E4*$T$14</f>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5">
+        <f t="shared" ref="R4:R12" si="9">E4*$R$14</f>
+        <v>0</v>
+      </c>
+      <c r="S4" s="5">
+        <f t="shared" ref="S4:S12" si="10">E4*$S$14</f>
+        <v>1</v>
+      </c>
+      <c r="T4" s="5">
+        <f t="shared" ref="T4:T12" si="11">E4*$T$14</f>
         <v>5</v>
       </c>
       <c r="V4">
-        <f t="shared" ref="V4:V12" si="9">N4*R4</f>
+        <f t="shared" ref="V4:V12" si="12">N4*R4</f>
         <v>0</v>
       </c>
       <c r="W4">
@@ -653,70 +657,70 @@
       <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>2</v>
       </c>
-      <c r="F5" s="3">
-        <f>COUNTIF(A:A,E5)</f>
-        <v>1</v>
-      </c>
-      <c r="G5" s="3">
-        <f>COUNTIF(B:B,E5)</f>
-        <v>1</v>
-      </c>
-      <c r="H5" s="3">
-        <f>COUNTIF(C:C,E5)</f>
-        <v>1</v>
-      </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4">
+      <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="K5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
         <f t="shared" si="1"/>
-        <v>0.1</v>
-      </c>
-      <c r="L5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
         <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="O5" s="4">
+      <c r="K5" s="3">
         <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="L5" s="3">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3">
+        <f t="shared" si="6"/>
+        <v>0.1</v>
+      </c>
+      <c r="O5" s="3">
+        <f t="shared" si="7"/>
         <v>1.0000000000000002E-2</v>
       </c>
-      <c r="P5" s="4">
-        <f t="shared" si="5"/>
+      <c r="P5" s="3">
+        <f t="shared" si="8"/>
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="S5" s="4">
-        <f t="shared" si="7"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S5" s="3">
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="T5" s="4">
-        <f t="shared" si="8"/>
+      <c r="T5" s="3">
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="V5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W5">
-        <f t="shared" ref="W5:X12" si="10">O5*S5</f>
+        <f t="shared" ref="W5:X12" si="13">O5*S5</f>
         <v>2.0000000000000004E-2</v>
       </c>
       <c r="X5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>1.0000000000000002E-2</v>
       </c>
       <c r="AA5">
@@ -736,70 +740,70 @@
       <c r="C6" s="1">
         <v>3</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>3</v>
       </c>
-      <c r="F6" s="5">
-        <f>COUNTIF(A:A,E6)</f>
-        <v>1</v>
-      </c>
-      <c r="G6" s="5">
-        <f>COUNTIF(B:B,E6)</f>
-        <v>1</v>
-      </c>
-      <c r="H6" s="5">
-        <f>COUNTIF(C:C,E6)</f>
-        <v>1</v>
-      </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6">
+      <c r="F6" s="4">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="K6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
         <f t="shared" si="1"/>
-        <v>0.1</v>
-      </c>
-      <c r="L6" s="6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4">
         <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="O6" s="6">
+      <c r="K6" s="5">
         <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="L6" s="5">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5">
+        <f t="shared" si="6"/>
+        <v>0.1</v>
+      </c>
+      <c r="O6" s="5">
+        <f t="shared" si="7"/>
         <v>1.0000000000000002E-2</v>
       </c>
-      <c r="P6" s="6">
-        <f t="shared" si="5"/>
+      <c r="P6" s="5">
+        <f t="shared" si="8"/>
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="S6" s="6">
-        <f t="shared" si="7"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S6" s="5">
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
-      <c r="T6" s="6">
-        <f t="shared" si="8"/>
+      <c r="T6" s="5">
+        <f t="shared" si="11"/>
         <v>15</v>
       </c>
       <c r="V6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>3.0000000000000006E-2</v>
       </c>
       <c r="X6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>1.5000000000000003E-2</v>
       </c>
       <c r="AA6">
@@ -819,70 +823,70 @@
       <c r="C7" s="1">
         <v>4</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>4</v>
       </c>
-      <c r="F7" s="3">
-        <f>COUNTIF(A:A,E7)</f>
-        <v>1</v>
-      </c>
-      <c r="G7" s="3">
-        <f>COUNTIF(B:B,E7)</f>
-        <v>1</v>
-      </c>
-      <c r="H7" s="3">
-        <f>COUNTIF(C:C,E7)</f>
-        <v>1</v>
-      </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4">
+      <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="K7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
         <f t="shared" si="1"/>
-        <v>0.1</v>
-      </c>
-      <c r="L7" s="4">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
         <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="O7" s="4">
+      <c r="K7" s="3">
         <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3">
+        <f t="shared" si="6"/>
+        <v>0.1</v>
+      </c>
+      <c r="O7" s="3">
+        <f t="shared" si="7"/>
         <v>1.0000000000000002E-2</v>
       </c>
-      <c r="P7" s="4">
-        <f t="shared" si="5"/>
+      <c r="P7" s="3">
+        <f t="shared" si="8"/>
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="S7" s="4">
-        <f t="shared" si="7"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S7" s="3">
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
-      <c r="T7" s="4">
-        <f t="shared" si="8"/>
+      <c r="T7" s="3">
+        <f t="shared" si="11"/>
         <v>20</v>
       </c>
       <c r="V7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>4.0000000000000008E-2</v>
       </c>
       <c r="X7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2.0000000000000004E-2</v>
       </c>
       <c r="AA7">
@@ -903,70 +907,70 @@
       <c r="C8" s="1">
         <v>5</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>5</v>
       </c>
-      <c r="F8" s="5">
-        <f>COUNTIF(A:A,E8)</f>
-        <v>1</v>
-      </c>
-      <c r="G8" s="5">
-        <f>COUNTIF(B:B,E8)</f>
-        <v>1</v>
-      </c>
-      <c r="H8" s="5">
-        <f>COUNTIF(C:C,E8)</f>
-        <v>1</v>
-      </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6">
+      <c r="F8" s="4">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="K8" s="6">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4">
         <f t="shared" si="1"/>
-        <v>0.1</v>
-      </c>
-      <c r="L8" s="6">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
         <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="O8" s="6">
+      <c r="K8" s="5">
         <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="L8" s="5">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5">
+        <f t="shared" si="6"/>
+        <v>0.1</v>
+      </c>
+      <c r="O8" s="5">
+        <f t="shared" si="7"/>
         <v>1.0000000000000002E-2</v>
       </c>
-      <c r="P8" s="6">
-        <f t="shared" si="5"/>
+      <c r="P8" s="5">
+        <f t="shared" si="8"/>
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="S8" s="6">
-        <f t="shared" si="7"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S8" s="5">
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
-      <c r="T8" s="6">
-        <f t="shared" si="8"/>
+      <c r="T8" s="5">
+        <f t="shared" si="11"/>
         <v>25</v>
       </c>
       <c r="V8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>5.000000000000001E-2</v>
       </c>
       <c r="X8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2.5000000000000005E-2</v>
       </c>
     </row>
@@ -980,71 +984,78 @@
       <c r="C9" s="1">
         <v>6</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>6</v>
       </c>
-      <c r="F9" s="3">
-        <f>COUNTIF(A:A,E9)</f>
-        <v>1</v>
-      </c>
-      <c r="G9" s="3">
-        <f>COUNTIF(B:B,E9)</f>
-        <v>1</v>
-      </c>
-      <c r="H9" s="3">
-        <f>COUNTIF(C:C,E9)</f>
-        <v>1</v>
-      </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4">
+      <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="K9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
         <f t="shared" si="1"/>
-        <v>0.1</v>
-      </c>
-      <c r="L9" s="4">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
         <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="O9" s="4">
+      <c r="K9" s="3">
         <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3">
+        <f t="shared" si="6"/>
+        <v>0.1</v>
+      </c>
+      <c r="O9" s="3">
+        <f t="shared" si="7"/>
         <v>1.0000000000000002E-2</v>
       </c>
-      <c r="P9" s="4">
-        <f t="shared" si="5"/>
+      <c r="P9" s="3">
+        <f t="shared" si="8"/>
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="S9" s="4">
-        <f t="shared" si="7"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S9" s="3">
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
-      <c r="T9" s="4">
-        <f t="shared" si="8"/>
+      <c r="T9" s="3">
+        <f t="shared" si="11"/>
         <v>30</v>
       </c>
       <c r="V9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>6.0000000000000012E-2</v>
       </c>
       <c r="X9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="AA9">
+        <f>(COUNT(A:A)-1)*(COUNT(B:B)-1)*(COUNT(C:C)-1)</f>
+        <v>512</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -1057,70 +1068,70 @@
       <c r="C10" s="1">
         <v>7</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>7</v>
       </c>
-      <c r="F10" s="5">
-        <f>COUNTIF(A:A,E10)</f>
-        <v>1</v>
-      </c>
-      <c r="G10" s="5">
-        <f>COUNTIF(B:B,E10)</f>
-        <v>1</v>
-      </c>
-      <c r="H10" s="5">
-        <f>COUNTIF(C:C,E10)</f>
-        <v>1</v>
-      </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6">
+      <c r="F10" s="4">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="K10" s="6">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4">
         <f t="shared" si="1"/>
-        <v>0.1</v>
-      </c>
-      <c r="L10" s="6">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4">
         <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6">
+        <v>1</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="O10" s="6">
+      <c r="K10" s="5">
         <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="L10" s="5">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5">
+        <f t="shared" si="6"/>
+        <v>0.1</v>
+      </c>
+      <c r="O10" s="5">
+        <f t="shared" si="7"/>
         <v>1.0000000000000002E-2</v>
       </c>
-      <c r="P10" s="6">
-        <f t="shared" si="5"/>
+      <c r="P10" s="5">
+        <f t="shared" si="8"/>
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="S10" s="6">
-        <f t="shared" si="7"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S10" s="5">
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
-      <c r="T10" s="6">
-        <f t="shared" si="8"/>
+      <c r="T10" s="5">
+        <f t="shared" si="11"/>
         <v>35</v>
       </c>
       <c r="V10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="X10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>3.500000000000001E-2</v>
       </c>
     </row>
@@ -1134,70 +1145,70 @@
       <c r="C11" s="1">
         <v>8</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>8</v>
       </c>
-      <c r="F11" s="3">
-        <f>COUNTIF(A:A,E11)</f>
-        <v>1</v>
-      </c>
-      <c r="G11" s="3">
-        <f>COUNTIF(B:B,E11)</f>
-        <v>1</v>
-      </c>
-      <c r="H11" s="3">
-        <f>COUNTIF(C:C,E11)</f>
-        <v>1</v>
-      </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4">
+      <c r="F11" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="K11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2">
         <f t="shared" si="1"/>
-        <v>0.1</v>
-      </c>
-      <c r="L11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
         <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="O11" s="4">
+      <c r="K11" s="3">
         <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3">
+        <f t="shared" si="6"/>
+        <v>0.1</v>
+      </c>
+      <c r="O11" s="3">
+        <f t="shared" si="7"/>
         <v>1.0000000000000002E-2</v>
       </c>
-      <c r="P11" s="4">
-        <f t="shared" si="5"/>
+      <c r="P11" s="3">
+        <f t="shared" si="8"/>
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="S11" s="4">
-        <f t="shared" si="7"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S11" s="3">
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
-      <c r="T11" s="4">
-        <f t="shared" si="8"/>
+      <c r="T11" s="3">
+        <f t="shared" si="11"/>
         <v>40</v>
       </c>
       <c r="V11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>8.0000000000000016E-2</v>
       </c>
       <c r="X11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>4.0000000000000008E-2</v>
       </c>
     </row>
@@ -1211,132 +1222,132 @@
       <c r="C12" s="1">
         <v>9</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>9</v>
       </c>
-      <c r="F12" s="5">
-        <f>COUNTIF(A:A,E12)</f>
-        <v>1</v>
-      </c>
-      <c r="G12" s="5">
-        <f>COUNTIF(B:B,E12)</f>
-        <v>1</v>
-      </c>
-      <c r="H12" s="5">
-        <f>COUNTIF(C:C,E12)</f>
-        <v>1</v>
-      </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6">
+      <c r="F12" s="4">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="K12" s="6">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4">
         <f t="shared" si="1"/>
-        <v>0.1</v>
-      </c>
-      <c r="L12" s="6">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4">
         <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6">
+        <v>1</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="O12" s="6">
+      <c r="K12" s="5">
         <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="L12" s="5">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5">
+        <f t="shared" si="6"/>
+        <v>0.1</v>
+      </c>
+      <c r="O12" s="5">
+        <f t="shared" si="7"/>
         <v>1.0000000000000002E-2</v>
       </c>
-      <c r="P12" s="6">
-        <f t="shared" si="5"/>
+      <c r="P12" s="5">
+        <f t="shared" si="8"/>
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="S12" s="6">
-        <f t="shared" si="7"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S12" s="5">
+        <f t="shared" si="10"/>
         <v>9</v>
       </c>
-      <c r="T12" s="6">
-        <f t="shared" si="8"/>
+      <c r="T12" s="5">
+        <f t="shared" si="11"/>
         <v>45</v>
       </c>
       <c r="V12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>9.0000000000000024E-2</v>
       </c>
       <c r="X12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>4.5000000000000012E-2</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="3">
-        <f>COUNTIF(A:A,E13)</f>
-        <v>1</v>
-      </c>
-      <c r="G13" s="3">
-        <f>COUNTIF(B:B,E13)</f>
-        <v>1</v>
-      </c>
-      <c r="H13" s="3">
-        <f>COUNTIF(C:C,E13)</f>
-        <v>1</v>
-      </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4">
+      <c r="F13" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="K13" s="4">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
         <f t="shared" si="1"/>
-        <v>0.1</v>
-      </c>
-      <c r="L13" s="4">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2">
         <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4">
-        <f t="shared" ref="N13" si="11">J13</f>
-        <v>0.1</v>
-      </c>
-      <c r="O13" s="4">
-        <f t="shared" ref="O13" si="12">J13*K13</f>
+        <v>1</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="L13" s="3">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3">
+        <f t="shared" ref="N13" si="14">J13</f>
+        <v>0.1</v>
+      </c>
+      <c r="O13" s="3">
+        <f t="shared" ref="O13" si="15">J13*K13</f>
         <v>1.0000000000000002E-2</v>
       </c>
-      <c r="P13" s="4">
-        <f t="shared" ref="P13" si="13">J13*K13*L13</f>
+      <c r="P13" s="3">
+        <f t="shared" ref="P13" si="16">J13*K13*L13</f>
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4">
-        <v>0</v>
-      </c>
-      <c r="S13" s="4">
-        <v>0</v>
-      </c>
-      <c r="T13" s="4">
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3">
+        <v>0</v>
+      </c>
+      <c r="S13" s="3">
+        <v>0</v>
+      </c>
+      <c r="T13" s="3">
         <f>AA6</f>
         <v>250</v>
       </c>
       <c r="V13">
-        <f t="shared" ref="V13" si="14">N13*R13</f>
+        <f t="shared" ref="V13" si="17">N13*R13</f>
         <v>0</v>
       </c>
       <c r="W13">
-        <f t="shared" ref="W13" si="15">O13*S13</f>
+        <f t="shared" ref="W13" si="18">O13*S13</f>
         <v>0</v>
       </c>
       <c r="X13">

</xml_diff>